<commit_message>
LAOZ - Commit por cambio sinesperados
</commit_message>
<xml_diff>
--- a/1 - Planeacion/2 - Estrategia/Lista de Chckeo Requerimientos.xlsx
+++ b/1 - Planeacion/2 - Estrategia/Lista de Chckeo Requerimientos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
+    <workbookView xWindow="240" yWindow="405" windowWidth="14805" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Checkeo Requerimientos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -604,10 +604,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>

</xml_diff>